<commit_message>
Add vehicle import functionality and new UI components; include sample data files
</commit_message>
<xml_diff>
--- a/rabbit_service_d_app/assets/sample_trailer_vehicle_data_rabbit.xlsx
+++ b/rabbit_service_d_app/assets/sample_trailer_vehicle_data_rabbit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\F-Drive-Data\MylexCompanyProjects\rabbit_services_project\rabbit_service_d_app\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A87F3B-166F-4249-857C-ED477D05735D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C6B397-F438-40DE-BC81-234DB4379BF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>vehicleType</t>
   </si>
@@ -64,12 +64,6 @@
     <t>CARRIER</t>
   </si>
   <si>
-    <t>25 Feb</t>
-  </si>
-  <si>
-    <t>BZDPT6650</t>
-  </si>
-  <si>
     <t>BZDPT</t>
   </si>
   <si>
@@ -77,6 +71,9 @@
   </si>
   <si>
     <t>AZXT6650G</t>
+  </si>
+  <si>
+    <t>BZ6650</t>
   </si>
 </sst>
 </file>
@@ -448,11 +445,12 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -502,25 +500,25 @@
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45741</v>
       </c>
       <c r="F2">
         <v>24000</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="I2">
         <v>1234</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K2" s="2">
         <v>45727</v>

</xml_diff>